<commit_message>
Removed timed file and correct saved sheet
</commit_message>
<xml_diff>
--- a/table_task_7.xlsx
+++ b/table_task_7.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Определение интервалов</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Макс. Значение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кол-во интервалов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ширина</t>
   </si>
 </sst>
 </file>
@@ -275,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V3" activeCellId="0" sqref="V3"/>
+      <selection pane="topLeft" activeCell="Y6" activeCellId="0" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -287,6 +293,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="5" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,6 +361,8 @@
         <v>0</v>
       </c>
       <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -422,6 +431,12 @@
       <c r="W2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="X2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -492,6 +507,13 @@
         <f aca="false">MAX(A1:T5)</f>
         <v>32</v>
       </c>
+      <c r="X3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <f aca="false">(W3-V3)/X3</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -619,7 +641,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V1:Y1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
#5 Finished subtasks 1 and 2 of task 7
</commit_message>
<xml_diff>
--- a/table_task_7.xlsx
+++ b/table_task_7.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="subtask1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Определение интервалов</t>
   </si>
@@ -35,6 +35,48 @@
   </si>
   <si>
     <t xml:space="preserve">Ширина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">границы интервалов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">интервалы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[2-5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[5-8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8-11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[11-14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[14-17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[17-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20-23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[23-26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[26-29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[29-32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Абсл. частота</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Накоп. частота</t>
   </si>
 </sst>
 </file>
@@ -44,11 +86,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,12 +113,22 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -116,7 +169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -143,29 +196,65 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Note" xfId="20"/>
+    <cellStyle name="Note 1" xfId="20"/>
+    <cellStyle name="Note 2" xfId="21"/>
+    <cellStyle name="Note" xfId="22"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -281,362 +370,550 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y6" activeCellId="0" sqref="Y6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA8" activeCellId="0" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="5" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="24.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="5" style="1" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="30" style="1" width="7.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
+      <c r="A1" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="n">
+      <c r="F1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="L1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="n">
+      <c r="L1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="Q1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="n">
+      <c r="Q1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="n">
+      <c r="I2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="n">
+      <c r="K2" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="n">
+      <c r="L2" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="M2" s="1" t="n">
+      <c r="M2" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="P2" s="1" t="n">
+      <c r="P2" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="Q2" s="1" t="n">
+      <c r="Q2" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="R2" s="1" t="n">
+      <c r="R2" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="S2" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="T2" s="1" t="n">
+      <c r="T2" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="V2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="B3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="n">
+      <c r="K3" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="L3" s="1" t="n">
+      <c r="L3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="M3" s="1" t="n">
+      <c r="M3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="N3" s="1" t="n">
+      <c r="N3" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="P3" s="1" t="n">
+      <c r="P3" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="Q3" s="1" t="n">
+      <c r="Q3" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="R3" s="1" t="n">
+      <c r="R3" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="S3" s="1" t="n">
+      <c r="S3" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="T3" s="1" t="n">
+      <c r="T3" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="4" t="n">
         <f aca="false">MIN(A1:T5)</f>
         <v>2</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="4" t="n">
         <f aca="false">MAX(A1:T5)</f>
         <v>32</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="4" t="n">
         <f aca="false">(W3-V3)/X3</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="I4" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="J4" s="1" t="n">
+      <c r="I4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="K4" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="L4" s="1" t="n">
+      <c r="L4" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="M4" s="1" t="n">
+      <c r="M4" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="N4" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="O4" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="P4" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="1" t="n">
+      <c r="N4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="R4" s="1" t="n">
+      <c r="R4" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="S4" s="1" t="n">
+      <c r="S4" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="T4" s="1" t="n">
+      <c r="T4" s="2" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="K5" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="L5" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="M5" s="1" t="n">
+      <c r="M5" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="N5" s="1" t="n">
+      <c r="N5" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="O5" s="1" t="n">
+      <c r="O5" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="P5" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q5" s="1" t="n">
+      <c r="P5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="R5" s="1" t="n">
+      <c r="R5" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="S5" s="1" t="n">
+      <c r="S5" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="T5" s="1" t="n">
+      <c r="T5" s="2" t="n">
         <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ7" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U8" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U8, A1:T5, "&lt;" &amp; U9)</f>
+        <v>2</v>
+      </c>
+      <c r="AB8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U9, A1:T5, "&lt;" &amp; U10)</f>
+        <v>6</v>
+      </c>
+      <c r="AC8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U10, A1:T5, "&lt;" &amp; U11)</f>
+        <v>3</v>
+      </c>
+      <c r="AD8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U11, A1:T5, "&lt;" &amp; U12)</f>
+        <v>10</v>
+      </c>
+      <c r="AE8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U12, A1:T5, "&lt;" &amp; U13)</f>
+        <v>23</v>
+      </c>
+      <c r="AF8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U13, A1:T5, "&lt;" &amp; U14)</f>
+        <v>18</v>
+      </c>
+      <c r="AG8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U14, A1:T5, "&lt;" &amp; U15)</f>
+        <v>23</v>
+      </c>
+      <c r="AH8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U15, A1:T5, "&lt;" &amp; U16)</f>
+        <v>8</v>
+      </c>
+      <c r="AI8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U16, A1:T5, "&lt;" &amp; U17)</f>
+        <v>5</v>
+      </c>
+      <c r="AJ8" s="8" t="n">
+        <f aca="false">COUNTIFS(A1:T5, "&gt;=" &amp; U17, A1:T5, "&lt;=" &amp; U18)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U9" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA9" s="8" t="n">
+        <f aca="false">AA8</f>
+        <v>2</v>
+      </c>
+      <c r="AB9" s="8" t="n">
+        <f aca="false">AB8+AA9</f>
+        <v>8</v>
+      </c>
+      <c r="AC9" s="8" t="n">
+        <f aca="false">AC8+AB9</f>
+        <v>11</v>
+      </c>
+      <c r="AD9" s="8" t="n">
+        <f aca="false">AD8+AC9</f>
+        <v>21</v>
+      </c>
+      <c r="AE9" s="8" t="n">
+        <f aca="false">AE8+AD9</f>
+        <v>44</v>
+      </c>
+      <c r="AF9" s="8" t="n">
+        <f aca="false">AF8+AE9</f>
+        <v>62</v>
+      </c>
+      <c r="AG9" s="8" t="n">
+        <f aca="false">AG8+AF9</f>
+        <v>85</v>
+      </c>
+      <c r="AH9" s="8" t="n">
+        <f aca="false">AH8+AG9</f>
+        <v>93</v>
+      </c>
+      <c r="AI9" s="8" t="n">
+        <f aca="false">AI8+AH9</f>
+        <v>98</v>
+      </c>
+      <c r="AJ9" s="8" t="n">
+        <f aca="false">AJ8+AI9</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U10" s="9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U11" s="9" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U12" s="9" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U13" s="9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U14" s="9" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U15" s="9" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U16" s="9" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U17" s="9" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U18" s="9" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#5 realisation of subtasks 3 and 4 to task 7
</commit_message>
<xml_diff>
--- a/table_task_7.xlsx
+++ b/table_task_7.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="subtask1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="subtask3" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">Определение интервалов</t>
   </si>
@@ -77,6 +78,30 @@
   </si>
   <si>
     <t xml:space="preserve">Накоп. частота</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мода</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Медиана</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выбороч. ср.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумма кв-ов отклон-ия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выборочное среднекв. Отклонение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кв. отклон-ия от ср.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Исправленное среднекв. Отклонение</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -169,7 +194,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,8 +227,11 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,8 +272,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="23" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -254,7 +294,8 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Note 1" xfId="20"/>
     <cellStyle name="Note 2" xfId="21"/>
-    <cellStyle name="Note" xfId="22"/>
+    <cellStyle name="Note 3" xfId="22"/>
+    <cellStyle name="Note 4" xfId="23"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -372,8 +413,8 @@
   </sheetPr>
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA8" activeCellId="0" sqref="AA8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -388,7 +429,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="14.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="5.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="30" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="30" style="1" width="7.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,4 +969,821 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:W13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V4" activeCellId="0" sqref="V4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="24.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="35.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="16.74"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="P1" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S1" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="T1" s="2" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>31</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="11" t="n">
+        <f aca="false">MODE(A1:T5)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="11" t="n">
+        <f aca="false">MEDIAN(A1:T5)</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="S4" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="11" t="n">
+        <f aca="false">AVERAGE(A1:T5)</f>
+        <v>17.29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="K5" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="W5" s="11" t="n">
+        <f aca="false">SUM(A7:T11)</f>
+        <v>3322.59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="W6" s="11" t="n">
+        <f aca="false">SQRT(W5 / 100)</f>
+        <v>5.76419118350528</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="n">
+        <f aca="false">(A1 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <f aca="false">(B1 - $W$4) ^ 2</f>
+        <v>18.4041</v>
+      </c>
+      <c r="C7" s="11" t="n">
+        <f aca="false">(C1 - $W$4) ^ 2</f>
+        <v>114.7041</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <f aca="false">(D1 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <f aca="false">(E1 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <f aca="false">(F1 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <f aca="false">(G1 - $W$4) ^ 2</f>
+        <v>45.0241</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <f aca="false">(H1 - $W$4) ^ 2</f>
+        <v>32.6041</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <f aca="false">(I1 - $W$4) ^ 2</f>
+        <v>0.504100000000001</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <f aca="false">(J1 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="K7" s="11" t="n">
+        <f aca="false">(K1 - $W$4) ^ 2</f>
+        <v>216.3841</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <f aca="false">(L1 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <f aca="false">(M1 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="N7" s="11" t="n">
+        <f aca="false">(N1 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="O7" s="11" t="n">
+        <f aca="false">(O1 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="P7" s="11" t="n">
+        <f aca="false">(P1 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="Q7" s="11" t="n">
+        <f aca="false">(Q1 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="R7" s="11" t="n">
+        <f aca="false">(R1 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="S7" s="11" t="n">
+        <f aca="false">(S1 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="T7" s="11" t="n">
+        <f aca="false">(T1 - $W$4) ^ 2</f>
+        <v>45.0241</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="W7" s="11" t="n">
+        <f aca="false">SQRT(W5 / 99)</f>
+        <v>5.79323011380656</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="n">
+        <f aca="false">(A2 - $W$4) ^ 2</f>
+        <v>105.8841</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <f aca="false">(B2 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="C8" s="11" t="n">
+        <f aca="false">(C2 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <f aca="false">(D2 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="E8" s="11" t="n">
+        <f aca="false">(E2 - $W$4) ^ 2</f>
+        <v>75.8641</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <f aca="false">(F2 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <f aca="false">(G2 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <f aca="false">(H2 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="I8" s="11" t="n">
+        <f aca="false">(I2 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="J8" s="11" t="n">
+        <f aca="false">(J2 - $W$4) ^ 2</f>
+        <v>32.6041</v>
+      </c>
+      <c r="K8" s="11" t="n">
+        <f aca="false">(K2 - $W$4) ^ 2</f>
+        <v>45.0241</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <f aca="false">(L2 - $W$4) ^ 2</f>
+        <v>0.504100000000001</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <f aca="false">(M2 - $W$4) ^ 2</f>
+        <v>59.4441</v>
+      </c>
+      <c r="N8" s="11" t="n">
+        <f aca="false">(N2 - $W$4) ^ 2</f>
+        <v>0.504100000000001</v>
+      </c>
+      <c r="O8" s="11" t="n">
+        <f aca="false">(O2 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="P8" s="11" t="n">
+        <f aca="false">(P2 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="Q8" s="11" t="n">
+        <f aca="false">(Q2 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="R8" s="11" t="n">
+        <f aca="false">(R2 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="S8" s="11" t="n">
+        <f aca="false">(S2 - $W$4) ^ 2</f>
+        <v>105.8841</v>
+      </c>
+      <c r="T8" s="11" t="n">
+        <f aca="false">(T2 - $W$4) ^ 2</f>
+        <v>187.9641</v>
+      </c>
+      <c r="U8" s="12"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="n">
+        <f aca="false">(A3 - $W$4) ^ 2</f>
+        <v>0.504100000000001</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <f aca="false">(B3 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <f aca="false">(C3 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <f aca="false">(D3 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="E9" s="11" t="n">
+        <f aca="false">(E3 - $W$4) ^ 2</f>
+        <v>151.0441</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <f aca="false">(F3 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <f aca="false">(G3 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="H9" s="11" t="n">
+        <f aca="false">(H3 - $W$4) ^ 2</f>
+        <v>39.5641</v>
+      </c>
+      <c r="I9" s="11" t="n">
+        <f aca="false">(I3 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="J9" s="11" t="n">
+        <f aca="false">(J3 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <f aca="false">(K3 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="L9" s="11" t="n">
+        <f aca="false">(L3 - $W$4) ^ 2</f>
+        <v>204.2041</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <f aca="false">(M3 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <f aca="false">(N3 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="O9" s="11" t="n">
+        <f aca="false">(O3 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <f aca="false">(P3 - $W$4) ^ 2</f>
+        <v>105.8841</v>
+      </c>
+      <c r="Q9" s="11" t="n">
+        <f aca="false">(Q3 - $W$4) ^ 2</f>
+        <v>59.4441</v>
+      </c>
+      <c r="R9" s="11" t="n">
+        <f aca="false">(R3 - $W$4) ^ 2</f>
+        <v>18.4041</v>
+      </c>
+      <c r="S9" s="11" t="n">
+        <f aca="false">(S3 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="T9" s="11" t="n">
+        <f aca="false">(T3 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="U9" s="12"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="n">
+        <f aca="false">(A4 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <f aca="false">(B4 - $W$4) ^ 2</f>
+        <v>27.9841</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <f aca="false">(C4 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <f aca="false">(D4 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="E10" s="11" t="n">
+        <f aca="false">(E4 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <f aca="false">(F4 - $W$4) ^ 2</f>
+        <v>22.1841</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <f aca="false">(G4 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="H10" s="11" t="n">
+        <f aca="false">(H4 - $W$4) ^ 2</f>
+        <v>105.8841</v>
+      </c>
+      <c r="I10" s="11" t="n">
+        <f aca="false">(I4 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="J10" s="11" t="n">
+        <f aca="false">(J4 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="K10" s="11" t="n">
+        <f aca="false">(K4 - $W$4) ^ 2</f>
+        <v>7.3441</v>
+      </c>
+      <c r="L10" s="11" t="n">
+        <f aca="false">(L4 - $W$4) ^ 2</f>
+        <v>75.8641</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <f aca="false">(M4 - $W$4) ^ 2</f>
+        <v>0.0840999999999995</v>
+      </c>
+      <c r="N10" s="11" t="n">
+        <f aca="false">(N4 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="O10" s="11" t="n">
+        <f aca="false">(O4 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="P10" s="11" t="n">
+        <f aca="false">(P4 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="Q10" s="11" t="n">
+        <f aca="false">(Q4 - $W$4) ^ 2</f>
+        <v>53.1441</v>
+      </c>
+      <c r="R10" s="11" t="n">
+        <f aca="false">(R4 - $W$4) ^ 2</f>
+        <v>75.8641</v>
+      </c>
+      <c r="S10" s="11" t="n">
+        <f aca="false">(S4 - $W$4) ^ 2</f>
+        <v>27.9841</v>
+      </c>
+      <c r="T10" s="11" t="n">
+        <f aca="false">(T4 - $W$4) ^ 2</f>
+        <v>68.7241</v>
+      </c>
+      <c r="U10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="n">
+        <f aca="false">(A5 - $W$4) ^ 2</f>
+        <v>27.9841</v>
+      </c>
+      <c r="B11" s="11" t="n">
+        <f aca="false">(B5 - $W$4) ^ 2</f>
+        <v>39.5641</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <f aca="false">(C5 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <f aca="false">(D5 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="E11" s="11" t="n">
+        <f aca="false">(E5 - $W$4) ^ 2</f>
+        <v>18.4041</v>
+      </c>
+      <c r="F11" s="11" t="n">
+        <f aca="false">(F5 - $W$4) ^ 2</f>
+        <v>5.2441</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">(G5 - $W$4) ^ 2</f>
+        <v>233.7841</v>
+      </c>
+      <c r="H11" s="11" t="n">
+        <f aca="false">(H5 - $W$4) ^ 2</f>
+        <v>127.4641</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <f aca="false">(I5 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="J11" s="11" t="n">
+        <f aca="false">(J5 - $W$4) ^ 2</f>
+        <v>68.7241</v>
+      </c>
+      <c r="K11" s="11" t="n">
+        <f aca="false">(K5 - $W$4) ^ 2</f>
+        <v>32.6041</v>
+      </c>
+      <c r="L11" s="11" t="n">
+        <f aca="false">(L5 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="M11" s="11" t="n">
+        <f aca="false">(M5 - $W$4) ^ 2</f>
+        <v>1.6641</v>
+      </c>
+      <c r="N11" s="11" t="n">
+        <f aca="false">(N5 - $W$4) ^ 2</f>
+        <v>13.7641</v>
+      </c>
+      <c r="O11" s="11" t="n">
+        <f aca="false">(O5 - $W$4) ^ 2</f>
+        <v>39.5641</v>
+      </c>
+      <c r="P11" s="11" t="n">
+        <f aca="false">(P5 - $W$4) ^ 2</f>
+        <v>10.8241</v>
+      </c>
+      <c r="Q11" s="11" t="n">
+        <f aca="false">(Q5 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="R11" s="11" t="n">
+        <f aca="false">(R5 - $W$4) ^ 2</f>
+        <v>2.9241</v>
+      </c>
+      <c r="S11" s="11" t="n">
+        <f aca="false">(S5 - $W$4) ^ 2</f>
+        <v>114.7041</v>
+      </c>
+      <c r="T11" s="11" t="n">
+        <f aca="false">(T5 - $W$4) ^ 2</f>
+        <v>27.9841</v>
+      </c>
+      <c r="U11" s="12"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="U7:U11"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>